<commit_message>
Check a title of a collection.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase.xlsx
+++ b/src/main/resources/TestCase.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="531">
   <si>
     <t>검색창</t>
   </si>
@@ -1673,10 +1673,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>goto_direct</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>academic section</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1780,342 +1776,350 @@
     <t>영화 정보</t>
   </si>
   <si>
+    <t>소프트웨어 정보</t>
+  </si>
+  <si>
+    <t>문화재 정보</t>
+  </si>
+  <si>
+    <t>증권 정보</t>
+  </si>
+  <si>
+    <t>만화정보</t>
+  </si>
+  <si>
+    <t>'연세대학교' 컨텐츠검색</t>
+  </si>
+  <si>
+    <t>민원정보</t>
+  </si>
+  <si>
+    <t>ds section</t>
+  </si>
+  <si>
+    <t>단위변환</t>
+  </si>
+  <si>
+    <t>지역번호 검색</t>
+  </si>
+  <si>
+    <t>'프라하의 연인' 방송정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플래시인기게임</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>단위환산, 5cm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>광주지역번호, 지역번호051</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스폰서링크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>블로그</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>책 본문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>카페</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동차 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>'SCH-W550' 쇼핑정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shopping_info section sh_shop_top</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>'SCH-W770' 쇼핑정보, 'LG-KU9100' 쇼핑정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>'장르별 플래시게임' 컨텐츠검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbplus section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애니메이션 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해외명소 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>요리 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음식재료 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 과학의 초전자포</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파전, 김치찜, 벨기에와플, 명란</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>치즈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뮤지컬 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뮤지컬공연 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>골든 리트리버, 프랑스 애견</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애견 주거, 강아지 영양, 강아지 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강아지 탈모증, 강아지 눈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애견 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애견관리 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애견질병 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbplus db_cols section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자연도감</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ndic section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사전</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>날씨 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스포츠 경기일정 다이렉트검색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dbplus festival section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>축제·행사 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_info section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_dummy section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>추천게임 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바로가기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>health_info section sh_health_top</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>의학 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nimage section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kinn section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지식iN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>land section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>region section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nmovie section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>동영상</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>music section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음악</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nxalbum section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>news section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뉴스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nsite section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사이트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>section movie_recomm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>movie_theater section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화관 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qna section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shopping_item section sh_shop_top</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shopping_list section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지식쇼핑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>webdoc section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹문서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>people_info section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플러스링크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>goto_direct section</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>영화 정보</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>소프트웨어 정보</t>
-  </si>
-  <si>
-    <t>문화재 정보</t>
-  </si>
-  <si>
-    <t>증권 정보</t>
-  </si>
-  <si>
-    <t>만화정보</t>
-  </si>
-  <si>
-    <t>'연세대학교' 컨텐츠검색</t>
-  </si>
-  <si>
-    <t>민원정보</t>
-  </si>
-  <si>
-    <t>ds section</t>
-  </si>
-  <si>
-    <t>단위변환</t>
-  </si>
-  <si>
-    <t>지역번호 검색</t>
-  </si>
-  <si>
-    <t>'프라하의 연인' 방송정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>플래시인기게임</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>단위환산, 5cm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>광주지역번호, 지역번호051</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>전문정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스폰서링크</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>블로그</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>책</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>책 본문</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>카페</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>자동차 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>'SCH-W550' 쇼핑정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shopping_info section sh_shop_top</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>'SCH-W770' 쇼핑정보, 'LG-KU9100' 쇼핑정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>'장르별 플래시게임' 컨텐츠검색</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>dbplus section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>애니메이션 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>해외명소 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>요리 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>음식재료 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>어떤 과학의 초전자포</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>파전, 김치찜, 벨기에와플, 명란</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>치즈</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>뮤지컬 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>뮤지컬공연 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>골든 리트리버, 프랑스 애견</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>애견 주거, 강아지 영양, 강아지 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>강아지 탈모증, 강아지 눈</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>애견 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>애견관리 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>애견질병 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>dbplus db_cols section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>자연도감</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ndic section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사전</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>날씨 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스포츠 경기일정 다이렉트검색</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>dbplus festival section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>축제·행사 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>축제·행사 스마트파인더™</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>game_info section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게임 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>goto_direct</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>game_dummy section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천게임 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>바로가기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>health_info section sh_health_top</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>의학 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nimage section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>kinn section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지식iN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>land section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부동산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>region section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지도</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nmovie section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>동영상</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>music section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>음악</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nxalbum section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>news section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>뉴스</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nsite section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사이트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>section movie_recomm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie_theater section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천영화 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화관 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>qna section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레시피 스마트파인더 ™</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shopping_item section sh_shop_top</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shopping_list section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지식쇼핑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>webdoc section</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>웹문서</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>people_info section</t>
+    <t>영화 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시퀀스검색 ™ 레시피 스마트파인더</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시퀀스검색 ™ 축제·행사 스마트파인더</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>goto_direct section</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3653,54 +3657,66 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3709,18 +3725,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4842,13 +4846,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D14:N14"/>
-    <mergeCell ref="D22:N22"/>
-    <mergeCell ref="D18:N18"/>
-    <mergeCell ref="D17:N17"/>
-    <mergeCell ref="D23:N23"/>
-    <mergeCell ref="D16:N16"/>
-    <mergeCell ref="D15:N15"/>
     <mergeCell ref="D12:N12"/>
     <mergeCell ref="D21:N21"/>
     <mergeCell ref="D25:N25"/>
@@ -4865,6 +4862,13 @@
     <mergeCell ref="D13:N13"/>
     <mergeCell ref="D20:N20"/>
     <mergeCell ref="D19:N19"/>
+    <mergeCell ref="D14:N14"/>
+    <mergeCell ref="D22:N22"/>
+    <mergeCell ref="D18:N18"/>
+    <mergeCell ref="D17:N17"/>
+    <mergeCell ref="D23:N23"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="D15:N15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4938,7 +4942,7 @@
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="168" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -4966,7 +4970,7 @@
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="158"/>
+      <c r="B6" s="163"/>
       <c r="C6" s="13" t="s">
         <v>42</v>
       </c>
@@ -4992,8 +4996,8 @@
       </c>
     </row>
     <row r="7" spans="2:11" s="99" customFormat="1">
-      <c r="B7" s="158"/>
-      <c r="C7" s="157" t="s">
+      <c r="B7" s="163"/>
+      <c r="C7" s="167" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="92" t="s">
@@ -5012,8 +5016,8 @@
       <c r="K7" s="98"/>
     </row>
     <row r="8" spans="2:11" s="99" customFormat="1">
-      <c r="B8" s="158"/>
-      <c r="C8" s="157"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="167"/>
       <c r="D8" s="92" t="s">
         <v>2</v>
       </c>
@@ -5030,7 +5034,7 @@
       <c r="K8" s="98"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="163" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -5060,7 +5064,7 @@
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="158"/>
+      <c r="B10" s="163"/>
       <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
@@ -5086,7 +5090,7 @@
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="158" t="s">
+      <c r="B11" s="163" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -5116,7 +5120,7 @@
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="158"/>
+      <c r="B12" s="163"/>
       <c r="C12" s="13" t="s">
         <v>51</v>
       </c>
@@ -5142,7 +5146,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" s="99" customFormat="1">
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="163" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="92" t="s">
@@ -5164,7 +5168,7 @@
       <c r="K13" s="98"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="158"/>
+      <c r="B14" s="163"/>
       <c r="C14" s="13" t="s">
         <v>63</v>
       </c>
@@ -5190,7 +5194,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="25.5">
-      <c r="B15" s="158"/>
+      <c r="B15" s="163"/>
       <c r="C15" s="13" t="s">
         <v>65</v>
       </c>
@@ -5218,10 +5222,10 @@
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="163" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="163" t="s">
+      <c r="C16" s="160" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -5230,7 +5234,7 @@
       <c r="E16" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="156" t="s">
+      <c r="F16" s="166" t="s">
         <v>71</v>
       </c>
       <c r="G16" s="90" t="s">
@@ -5248,15 +5252,15 @@
       </c>
     </row>
     <row r="17" spans="2:11" s="99" customFormat="1">
-      <c r="B17" s="158"/>
-      <c r="C17" s="163"/>
+      <c r="B17" s="163"/>
+      <c r="C17" s="160"/>
       <c r="D17" s="92" t="s">
         <v>60</v>
       </c>
       <c r="E17" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="156"/>
+      <c r="F17" s="166"/>
       <c r="G17" s="95"/>
       <c r="H17" s="96"/>
       <c r="I17" s="96"/>
@@ -5264,15 +5268,15 @@
       <c r="K17" s="98"/>
     </row>
     <row r="18" spans="2:11" ht="25.5">
-      <c r="B18" s="158"/>
-      <c r="C18" s="163"/>
+      <c r="B18" s="163"/>
+      <c r="C18" s="160"/>
       <c r="D18" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="156"/>
+      <c r="F18" s="166"/>
       <c r="G18" s="90" t="s">
         <v>325</v>
       </c>
@@ -5288,8 +5292,8 @@
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="158"/>
-      <c r="C19" s="163" t="s">
+      <c r="B19" s="163"/>
+      <c r="C19" s="160" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -5314,8 +5318,8 @@
       </c>
     </row>
     <row r="20" spans="2:11" ht="25.5">
-      <c r="B20" s="158"/>
-      <c r="C20" s="164"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="157"/>
       <c r="D20" s="13" t="s">
         <v>47</v>
       </c>
@@ -5338,7 +5342,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" s="99" customFormat="1">
-      <c r="B21" s="161" t="s">
+      <c r="B21" s="165" t="s">
         <v>77</v>
       </c>
       <c r="C21" s="92" t="s">
@@ -5360,8 +5364,8 @@
       <c r="K21" s="98"/>
     </row>
     <row r="22" spans="2:11" s="99" customFormat="1" ht="25.5">
-      <c r="B22" s="161"/>
-      <c r="C22" s="164" t="s">
+      <c r="B22" s="165"/>
+      <c r="C22" s="157" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="92" t="s">
@@ -5380,8 +5384,8 @@
       <c r="K22" s="98"/>
     </row>
     <row r="23" spans="2:11" s="99" customFormat="1" ht="25.5">
-      <c r="B23" s="161"/>
-      <c r="C23" s="164"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="157"/>
       <c r="D23" s="92" t="s">
         <v>52</v>
       </c>
@@ -5398,7 +5402,7 @@
       <c r="K23" s="98"/>
     </row>
     <row r="24" spans="2:11" s="99" customFormat="1" ht="25.5">
-      <c r="B24" s="161"/>
+      <c r="B24" s="165"/>
       <c r="C24" s="100" t="s">
         <v>82</v>
       </c>
@@ -5418,7 +5422,7 @@
       <c r="K24" s="98"/>
     </row>
     <row r="25" spans="2:11" s="99" customFormat="1">
-      <c r="B25" s="161"/>
+      <c r="B25" s="165"/>
       <c r="C25" s="92" t="s">
         <v>84</v>
       </c>
@@ -5438,7 +5442,7 @@
       <c r="K25" s="98"/>
     </row>
     <row r="26" spans="2:11" s="99" customFormat="1">
-      <c r="B26" s="161"/>
+      <c r="B26" s="165"/>
       <c r="C26" s="92" t="s">
         <v>87</v>
       </c>
@@ -5458,10 +5462,10 @@
       <c r="K26" s="98"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="158" t="s">
+      <c r="B27" s="163" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="163" t="s">
+      <c r="C27" s="160" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -5488,8 +5492,8 @@
       </c>
     </row>
     <row r="28" spans="2:11" s="99" customFormat="1">
-      <c r="B28" s="158"/>
-      <c r="C28" s="163"/>
+      <c r="B28" s="163"/>
+      <c r="C28" s="160"/>
       <c r="D28" s="92" t="s">
         <v>47</v>
       </c>
@@ -5506,8 +5510,8 @@
       <c r="K28" s="98"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="158"/>
-      <c r="C29" s="163"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="160"/>
       <c r="D29" s="13" t="s">
         <v>47</v>
       </c>
@@ -5530,7 +5534,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" s="99" customFormat="1">
-      <c r="B30" s="158" t="s">
+      <c r="B30" s="163" t="s">
         <v>95</v>
       </c>
       <c r="C30" s="92" t="s">
@@ -5552,7 +5556,7 @@
       <c r="K30" s="98"/>
     </row>
     <row r="31" spans="2:11" s="99" customFormat="1" ht="13.5" thickBot="1">
-      <c r="B31" s="160"/>
+      <c r="B31" s="164"/>
       <c r="C31" s="101" t="s">
         <v>98</v>
       </c>
@@ -5570,10 +5574,10 @@
       <c r="K31" s="107"/>
     </row>
     <row r="32" spans="2:11" hidden="1">
-      <c r="B32" s="165" t="s">
+      <c r="B32" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="167" t="s">
+      <c r="C32" s="159" t="s">
         <v>101</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -5591,8 +5595,8 @@
       <c r="J32" s="45"/>
     </row>
     <row r="33" spans="2:10" hidden="1">
-      <c r="B33" s="164"/>
-      <c r="C33" s="163"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="160"/>
       <c r="D33" s="13" t="s">
         <v>47</v>
       </c>
@@ -5606,8 +5610,8 @@
       <c r="J33" s="39"/>
     </row>
     <row r="34" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B34" s="164"/>
-      <c r="C34" s="163" t="s">
+      <c r="B34" s="157"/>
+      <c r="C34" s="160" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="13" t="s">
@@ -5625,8 +5629,8 @@
       <c r="J34" s="39"/>
     </row>
     <row r="35" spans="2:10" hidden="1">
-      <c r="B35" s="164"/>
-      <c r="C35" s="163"/>
+      <c r="B35" s="157"/>
+      <c r="C35" s="160"/>
       <c r="D35" s="13" t="s">
         <v>47</v>
       </c>
@@ -5640,8 +5644,8 @@
       <c r="J35" s="39"/>
     </row>
     <row r="36" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B36" s="164"/>
-      <c r="C36" s="163" t="s">
+      <c r="B36" s="157"/>
+      <c r="C36" s="160" t="s">
         <v>107</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -5659,8 +5663,8 @@
       <c r="J36" s="39"/>
     </row>
     <row r="37" spans="2:10" hidden="1">
-      <c r="B37" s="164"/>
-      <c r="C37" s="163"/>
+      <c r="B37" s="157"/>
+      <c r="C37" s="160"/>
       <c r="D37" s="13" t="s">
         <v>47</v>
       </c>
@@ -5674,8 +5678,8 @@
       <c r="J37" s="39"/>
     </row>
     <row r="38" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B38" s="164"/>
-      <c r="C38" s="163" t="s">
+      <c r="B38" s="157"/>
+      <c r="C38" s="160" t="s">
         <v>109</v>
       </c>
       <c r="D38" s="13" t="s">
@@ -5693,8 +5697,8 @@
       <c r="J38" s="39"/>
     </row>
     <row r="39" spans="2:10" hidden="1">
-      <c r="B39" s="164"/>
-      <c r="C39" s="163"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="160"/>
       <c r="D39" s="13" t="s">
         <v>47</v>
       </c>
@@ -5708,8 +5712,8 @@
       <c r="J39" s="39"/>
     </row>
     <row r="40" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B40" s="164"/>
-      <c r="C40" s="163" t="s">
+      <c r="B40" s="157"/>
+      <c r="C40" s="160" t="s">
         <v>111</v>
       </c>
       <c r="D40" s="13" t="s">
@@ -5727,8 +5731,8 @@
       <c r="J40" s="39"/>
     </row>
     <row r="41" spans="2:10" hidden="1">
-      <c r="B41" s="164"/>
-      <c r="C41" s="163"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="160"/>
       <c r="D41" s="13" t="s">
         <v>47</v>
       </c>
@@ -5742,8 +5746,8 @@
       <c r="J41" s="39"/>
     </row>
     <row r="42" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B42" s="164"/>
-      <c r="C42" s="163" t="s">
+      <c r="B42" s="157"/>
+      <c r="C42" s="160" t="s">
         <v>113</v>
       </c>
       <c r="D42" s="13" t="s">
@@ -5761,8 +5765,8 @@
       <c r="J42" s="39"/>
     </row>
     <row r="43" spans="2:10" ht="17.25" hidden="1" customHeight="1" thickBot="1">
-      <c r="B43" s="166"/>
-      <c r="C43" s="168"/>
+      <c r="B43" s="158"/>
+      <c r="C43" s="161"/>
       <c r="D43" s="20" t="s">
         <v>47</v>
       </c>
@@ -5904,6 +5908,21 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="B32:B43"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
@@ -5911,21 +5930,6 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C43"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G1:I1048576 J1:J2 J4:J1048576 K4">
@@ -5956,9 +5960,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6034,10 +6038,10 @@
         <v>133</v>
       </c>
       <c r="E5" s="139" t="s">
-        <v>414</v>
+        <v>525</v>
       </c>
       <c r="F5" s="139" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="44" t="s">
@@ -6058,7 +6062,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="170" t="s">
         <v>134</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -6068,10 +6072,10 @@
         <v>136</v>
       </c>
       <c r="E6" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F6" s="141" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="48" t="s">
@@ -6093,7 +6097,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="178"/>
+      <c r="B7" s="172"/>
       <c r="C7" s="14" t="s">
         <v>137</v>
       </c>
@@ -6101,10 +6105,10 @@
         <v>138</v>
       </c>
       <c r="E7" s="141" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F7" s="141" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="48" t="s">
@@ -6125,7 +6129,7 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="178"/>
+      <c r="B8" s="172"/>
       <c r="C8" s="51" t="s">
         <v>139</v>
       </c>
@@ -6133,10 +6137,10 @@
         <v>140</v>
       </c>
       <c r="E8" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F8" s="141" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="48" t="s">
@@ -6158,7 +6162,7 @@
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="178"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="51" t="s">
         <v>141</v>
       </c>
@@ -6166,10 +6170,10 @@
         <v>142</v>
       </c>
       <c r="E9" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F9" s="141" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G9" s="47" t="s">
         <v>143</v>
@@ -6193,7 +6197,7 @@
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="172"/>
       <c r="C10" s="51" t="s">
         <v>144</v>
       </c>
@@ -6201,10 +6205,10 @@
         <v>145</v>
       </c>
       <c r="E10" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F10" s="141" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="48" t="s">
@@ -6225,7 +6229,7 @@
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="178"/>
+      <c r="B11" s="172"/>
       <c r="C11" s="51" t="s">
         <v>146</v>
       </c>
@@ -6233,10 +6237,10 @@
         <v>147</v>
       </c>
       <c r="E11" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F11" s="141" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="48" t="s">
@@ -6257,7 +6261,7 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="178"/>
+      <c r="B12" s="172"/>
       <c r="C12" s="51" t="s">
         <v>148</v>
       </c>
@@ -6265,10 +6269,10 @@
         <v>149</v>
       </c>
       <c r="E12" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F12" s="141" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G12" s="47"/>
       <c r="H12" s="48" t="s">
@@ -6289,7 +6293,7 @@
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="178"/>
+      <c r="B13" s="172"/>
       <c r="C13" s="51" t="s">
         <v>150</v>
       </c>
@@ -6297,10 +6301,10 @@
         <v>151</v>
       </c>
       <c r="E13" s="141" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F13" s="141" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G13" s="47" t="s">
         <v>152</v>
@@ -6323,7 +6327,7 @@
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="178"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="14" t="s">
         <v>153</v>
       </c>
@@ -6331,10 +6335,10 @@
         <v>154</v>
       </c>
       <c r="E14" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F14" s="141" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="48" t="s">
@@ -6355,7 +6359,7 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="178"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="51" t="s">
         <v>155</v>
       </c>
@@ -6363,10 +6367,10 @@
         <v>156</v>
       </c>
       <c r="E15" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F15" s="141" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="48" t="s">
@@ -6387,7 +6391,7 @@
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="178"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="51" t="s">
         <v>157</v>
       </c>
@@ -6395,10 +6399,10 @@
         <v>158</v>
       </c>
       <c r="E16" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F16" s="141" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="48" t="s">
@@ -6419,7 +6423,7 @@
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="178"/>
+      <c r="B17" s="172"/>
       <c r="C17" s="51" t="s">
         <v>159</v>
       </c>
@@ -6427,10 +6431,10 @@
         <v>160</v>
       </c>
       <c r="E17" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F17" s="141" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G17" s="47"/>
       <c r="H17" s="48" t="s">
@@ -6451,7 +6455,7 @@
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="178"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="51" t="s">
         <v>161</v>
       </c>
@@ -6459,10 +6463,10 @@
         <v>162</v>
       </c>
       <c r="E18" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F18" s="141" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="48" t="s">
@@ -6483,7 +6487,7 @@
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="178"/>
+      <c r="B19" s="172"/>
       <c r="C19" s="51" t="s">
         <v>164</v>
       </c>
@@ -6491,10 +6495,10 @@
         <v>165</v>
       </c>
       <c r="E19" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F19" s="141" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="48" t="s">
@@ -6515,18 +6519,18 @@
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="178"/>
+      <c r="B20" s="172"/>
       <c r="C20" s="51" t="s">
         <v>394</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E20" s="141" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F20" s="146" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="48"/>
@@ -6539,18 +6543,18 @@
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="178"/>
+      <c r="B21" s="172"/>
       <c r="C21" s="51" t="s">
         <v>411</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E21" s="141" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F21" s="141" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G21" s="47"/>
       <c r="H21" s="48"/>
@@ -6563,18 +6567,18 @@
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="177"/>
+      <c r="B22" s="171"/>
       <c r="C22" s="51" t="s">
         <v>409</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E22" s="141" t="s">
+        <v>448</v>
+      </c>
+      <c r="F22" s="141" t="s">
         <v>450</v>
-      </c>
-      <c r="F22" s="141" t="s">
-        <v>452</v>
       </c>
       <c r="G22" s="47"/>
       <c r="H22" s="48"/>
@@ -6587,7 +6591,7 @@
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="170" t="s">
         <v>166</v>
       </c>
       <c r="C23" s="51" t="s">
@@ -6597,10 +6601,10 @@
         <v>163</v>
       </c>
       <c r="E23" s="141" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F23" s="141" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G23" s="47"/>
       <c r="H23" s="48" t="s">
@@ -6621,7 +6625,7 @@
       <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="177"/>
+      <c r="B24" s="171"/>
       <c r="C24" s="51" t="s">
         <v>167</v>
       </c>
@@ -6629,10 +6633,10 @@
         <v>168</v>
       </c>
       <c r="E24" s="140" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F24" s="140" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G24" s="47"/>
       <c r="H24" s="48" t="s">
@@ -6653,20 +6657,20 @@
       <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="158" t="s">
+      <c r="B25" s="163" t="s">
         <v>169</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="175" t="s">
+      <c r="D25" s="169" t="s">
         <v>171</v>
       </c>
       <c r="E25" s="142" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F25" s="142" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G25" s="47"/>
       <c r="H25" s="48" t="s">
@@ -6687,13 +6691,13 @@
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="158"/>
+      <c r="B26" s="163"/>
       <c r="C26" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="175"/>
+      <c r="D26" s="169"/>
       <c r="E26" s="142" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F26" s="51" t="s">
         <v>172</v>
@@ -6717,16 +6721,16 @@
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="158"/>
+      <c r="B27" s="163"/>
       <c r="C27" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="D27" s="175"/>
+      <c r="D27" s="169"/>
       <c r="E27" s="142" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>173</v>
+        <v>524</v>
       </c>
       <c r="G27" s="47"/>
       <c r="H27" s="48" t="s">
@@ -6747,13 +6751,13 @@
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="158"/>
+      <c r="B28" s="163"/>
       <c r="C28" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="175"/>
+      <c r="D28" s="169"/>
       <c r="E28" s="142" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F28" s="51" t="s">
         <v>174</v>
@@ -6777,7 +6781,7 @@
       <c r="A29" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="158" t="s">
+      <c r="B29" s="163" t="s">
         <v>326</v>
       </c>
       <c r="C29" s="51" t="s">
@@ -6787,10 +6791,10 @@
         <v>176</v>
       </c>
       <c r="E29" s="140" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F29" s="140" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G29" s="47"/>
       <c r="H29" s="48" t="s">
@@ -6811,7 +6815,7 @@
       <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="158"/>
+      <c r="B30" s="163"/>
       <c r="C30" s="51" t="s">
         <v>177</v>
       </c>
@@ -6819,10 +6823,10 @@
         <v>178</v>
       </c>
       <c r="E30" s="140" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F30" s="140" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G30" s="47"/>
       <c r="H30" s="48" t="s">
@@ -6843,7 +6847,7 @@
       <c r="A31" s="1">
         <v>27</v>
       </c>
-      <c r="B31" s="169" t="s">
+      <c r="B31" s="173" t="s">
         <v>137</v>
       </c>
       <c r="C31" s="51" t="s">
@@ -6853,10 +6857,10 @@
         <v>180</v>
       </c>
       <c r="E31" s="141" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F31" s="141" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G31" s="47"/>
       <c r="H31" s="48" t="s">
@@ -6877,7 +6881,7 @@
       <c r="A32" s="1">
         <v>28</v>
       </c>
-      <c r="B32" s="159"/>
+      <c r="B32" s="168"/>
       <c r="C32" s="51" t="s">
         <v>181</v>
       </c>
@@ -6885,10 +6889,10 @@
         <v>182</v>
       </c>
       <c r="E32" s="141" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F32" s="141" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="48" t="s">
@@ -6909,7 +6913,7 @@
       <c r="A33" s="1">
         <v>29</v>
       </c>
-      <c r="B33" s="169" t="s">
+      <c r="B33" s="173" t="s">
         <v>183</v>
       </c>
       <c r="C33" s="51" t="s">
@@ -6919,10 +6923,10 @@
         <v>185</v>
       </c>
       <c r="E33" s="141" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F33" s="141" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="48" t="s">
@@ -6943,7 +6947,7 @@
       <c r="A34" s="1">
         <v>30</v>
       </c>
-      <c r="B34" s="171"/>
+      <c r="B34" s="174"/>
       <c r="C34" s="51" t="s">
         <v>186</v>
       </c>
@@ -6951,10 +6955,10 @@
         <v>187</v>
       </c>
       <c r="E34" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F34" s="141" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G34" s="47"/>
       <c r="H34" s="48" t="s">
@@ -6975,7 +6979,7 @@
       <c r="A35" s="1">
         <v>31</v>
       </c>
-      <c r="B35" s="171"/>
+      <c r="B35" s="174"/>
       <c r="C35" s="51" t="s">
         <v>188</v>
       </c>
@@ -6983,10 +6987,10 @@
         <v>189</v>
       </c>
       <c r="E35" s="141" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F35" s="141" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G35" s="47"/>
       <c r="H35" s="48" t="s">
@@ -7007,7 +7011,7 @@
       <c r="A36" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="169" t="s">
+      <c r="B36" s="173" t="s">
         <v>190</v>
       </c>
       <c r="C36" s="51" t="s">
@@ -7017,10 +7021,10 @@
         <v>192</v>
       </c>
       <c r="E36" s="141" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F36" s="141" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G36" s="47"/>
       <c r="H36" s="48" t="s">
@@ -7041,7 +7045,7 @@
       <c r="A37" s="1">
         <v>33</v>
       </c>
-      <c r="B37" s="171"/>
+      <c r="B37" s="174"/>
       <c r="C37" s="51" t="s">
         <v>193</v>
       </c>
@@ -7049,10 +7053,10 @@
         <v>194</v>
       </c>
       <c r="E37" s="141" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F37" s="141" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G37" s="47"/>
       <c r="H37" s="48" t="s">
@@ -7073,7 +7077,7 @@
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="171"/>
+      <c r="B38" s="174"/>
       <c r="C38" s="51" t="s">
         <v>195</v>
       </c>
@@ -7081,10 +7085,10 @@
         <v>196</v>
       </c>
       <c r="E38" s="141" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F38" s="141" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G38" s="47"/>
       <c r="H38" s="48" t="s">
@@ -7105,7 +7109,7 @@
       <c r="A39" s="1">
         <v>35</v>
       </c>
-      <c r="B39" s="169" t="s">
+      <c r="B39" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C39" s="51" t="s">
@@ -7115,10 +7119,10 @@
         <v>199</v>
       </c>
       <c r="E39" s="141" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F39" s="141" t="s">
-        <v>443</v>
+        <v>526</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="48" t="s">
@@ -7139,7 +7143,7 @@
       <c r="A40" s="1">
         <v>36</v>
       </c>
-      <c r="B40" s="171"/>
+      <c r="B40" s="174"/>
       <c r="C40" s="51" t="s">
         <v>200</v>
       </c>
@@ -7147,10 +7151,10 @@
         <v>201</v>
       </c>
       <c r="E40" s="141" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F40" s="141" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="G40" s="47"/>
       <c r="H40" s="48" t="s">
@@ -7171,7 +7175,7 @@
       <c r="A41" s="1">
         <v>37</v>
       </c>
-      <c r="B41" s="171"/>
+      <c r="B41" s="174"/>
       <c r="C41" s="51" t="s">
         <v>202</v>
       </c>
@@ -7179,10 +7183,10 @@
         <v>203</v>
       </c>
       <c r="E41" s="141" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F41" s="141" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="G41" s="47"/>
       <c r="H41" s="48" t="s">
@@ -7203,7 +7207,7 @@
       <c r="A42" s="1">
         <v>38</v>
       </c>
-      <c r="B42" s="169" t="s">
+      <c r="B42" s="173" t="s">
         <v>204</v>
       </c>
       <c r="C42" s="51" t="s">
@@ -7213,10 +7217,10 @@
         <v>205</v>
       </c>
       <c r="E42" s="141" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F42" s="146" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G42" s="47"/>
       <c r="H42" s="48" t="s">
@@ -7237,7 +7241,7 @@
       <c r="A43" s="1">
         <v>39</v>
       </c>
-      <c r="B43" s="171"/>
+      <c r="B43" s="174"/>
       <c r="C43" s="51" t="s">
         <v>206</v>
       </c>
@@ -7245,10 +7249,10 @@
         <v>207</v>
       </c>
       <c r="E43" s="141" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F43" s="146" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G43" s="47"/>
       <c r="H43" s="48" t="s">
@@ -7269,7 +7273,7 @@
       <c r="A44" s="1">
         <v>40</v>
       </c>
-      <c r="B44" s="169" t="s">
+      <c r="B44" s="173" t="s">
         <v>398</v>
       </c>
       <c r="C44" s="51" t="s">
@@ -7279,10 +7283,10 @@
         <v>399</v>
       </c>
       <c r="E44" s="141" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="F44" s="141" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="G44" s="47"/>
       <c r="H44" s="48"/>
@@ -7295,7 +7299,7 @@
       <c r="A45" s="1">
         <v>41</v>
       </c>
-      <c r="B45" s="171"/>
+      <c r="B45" s="174"/>
       <c r="C45" s="51" t="s">
         <v>402</v>
       </c>
@@ -7303,10 +7307,10 @@
         <v>400</v>
       </c>
       <c r="E45" s="141" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="F45" s="141" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="G45" s="47"/>
       <c r="H45" s="48"/>
@@ -7319,7 +7323,7 @@
       <c r="A46" s="1">
         <v>42</v>
       </c>
-      <c r="B46" s="169" t="s">
+      <c r="B46" s="173" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="51" t="s">
@@ -7329,10 +7333,10 @@
         <v>33</v>
       </c>
       <c r="E46" s="141" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F46" s="141" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="G46" s="47"/>
       <c r="H46" s="48" t="s">
@@ -7353,7 +7357,7 @@
       <c r="A47" s="1">
         <v>43</v>
       </c>
-      <c r="B47" s="171"/>
+      <c r="B47" s="174"/>
       <c r="C47" s="51" t="s">
         <v>34</v>
       </c>
@@ -7361,10 +7365,10 @@
         <v>35</v>
       </c>
       <c r="E47" s="141" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F47" s="141" t="s">
-        <v>492</v>
+        <v>529</v>
       </c>
       <c r="G47" s="47"/>
       <c r="H47" s="48" t="s">
@@ -7385,7 +7389,7 @@
       <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B48" s="169" t="s">
+      <c r="B48" s="173" t="s">
         <v>208</v>
       </c>
       <c r="C48" s="51" t="s">
@@ -7395,10 +7399,10 @@
         <v>210</v>
       </c>
       <c r="E48" s="141" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F48" s="141" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G48" s="47"/>
       <c r="H48" s="48" t="s">
@@ -7419,7 +7423,7 @@
       <c r="A49" s="1">
         <v>45</v>
       </c>
-      <c r="B49" s="171"/>
+      <c r="B49" s="174"/>
       <c r="C49" s="51" t="s">
         <v>211</v>
       </c>
@@ -7427,10 +7431,10 @@
         <v>212</v>
       </c>
       <c r="E49" s="141" t="s">
-        <v>495</v>
+        <v>530</v>
       </c>
       <c r="F49" s="141" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="G49" s="47"/>
       <c r="H49" s="48" t="s">
@@ -7451,7 +7455,7 @@
       <c r="A50" s="1">
         <v>46</v>
       </c>
-      <c r="B50" s="171"/>
+      <c r="B50" s="174"/>
       <c r="C50" s="51" t="s">
         <v>200</v>
       </c>
@@ -7459,10 +7463,10 @@
         <v>213</v>
       </c>
       <c r="E50" s="141" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F50" s="141" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G50" s="47"/>
       <c r="H50" s="48" t="s">
@@ -7483,7 +7487,7 @@
       <c r="A51" s="1">
         <v>47</v>
       </c>
-      <c r="B51" s="171"/>
+      <c r="B51" s="174"/>
       <c r="C51" s="51" t="s">
         <v>214</v>
       </c>
@@ -7491,10 +7495,10 @@
         <v>215</v>
       </c>
       <c r="E51" s="141" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F51" s="141" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G51" s="47"/>
       <c r="H51" s="48" t="s">
@@ -7515,7 +7519,7 @@
       <c r="A52" s="1">
         <v>48</v>
       </c>
-      <c r="B52" s="158" t="s">
+      <c r="B52" s="163" t="s">
         <v>216</v>
       </c>
       <c r="C52" s="51" t="s">
@@ -7525,10 +7529,10 @@
         <v>218</v>
       </c>
       <c r="E52" s="141" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F52" s="141" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="G52" s="47"/>
       <c r="H52" s="48" t="s">
@@ -7549,7 +7553,7 @@
       <c r="A53" s="1">
         <v>49</v>
       </c>
-      <c r="B53" s="158"/>
+      <c r="B53" s="163"/>
       <c r="C53" s="51" t="s">
         <v>219</v>
       </c>
@@ -7557,10 +7561,10 @@
         <v>220</v>
       </c>
       <c r="E53" s="140" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F53" s="141" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="G53" s="47"/>
       <c r="H53" s="48" t="s">
@@ -7581,7 +7585,7 @@
       <c r="A54" s="1">
         <v>50</v>
       </c>
-      <c r="B54" s="158"/>
+      <c r="B54" s="163"/>
       <c r="C54" s="51" t="s">
         <v>221</v>
       </c>
@@ -7589,10 +7593,10 @@
         <v>222</v>
       </c>
       <c r="E54" s="140" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F54" s="141" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="G54" s="47"/>
       <c r="H54" s="48" t="s">
@@ -7621,10 +7625,10 @@
         <v>224</v>
       </c>
       <c r="E55" s="141" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F55" s="141" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="G55" s="47"/>
       <c r="H55" s="48" t="s">
@@ -7645,7 +7649,7 @@
       <c r="A56" s="1">
         <v>52</v>
       </c>
-      <c r="B56" s="172" t="s">
+      <c r="B56" s="176" t="s">
         <v>346</v>
       </c>
       <c r="C56" s="130" t="s">
@@ -7655,10 +7659,10 @@
         <v>348</v>
       </c>
       <c r="E56" s="143" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F56" s="143" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G56" s="131"/>
       <c r="H56" s="132" t="s">
@@ -7679,7 +7683,7 @@
       <c r="A57" s="1">
         <v>53</v>
       </c>
-      <c r="B57" s="173"/>
+      <c r="B57" s="177"/>
       <c r="C57" s="130" t="s">
         <v>349</v>
       </c>
@@ -7687,10 +7691,10 @@
         <v>350</v>
       </c>
       <c r="E57" s="143" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F57" s="143" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G57" s="131"/>
       <c r="H57" s="132" t="s">
@@ -7711,7 +7715,7 @@
       <c r="A58" s="1">
         <v>54</v>
       </c>
-      <c r="B58" s="173"/>
+      <c r="B58" s="177"/>
       <c r="C58" s="130" t="s">
         <v>351</v>
       </c>
@@ -7719,10 +7723,10 @@
         <v>352</v>
       </c>
       <c r="E58" s="143" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F58" s="143" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G58" s="131"/>
       <c r="H58" s="132" t="s">
@@ -7743,7 +7747,7 @@
       <c r="A59" s="1">
         <v>55</v>
       </c>
-      <c r="B59" s="174"/>
+      <c r="B59" s="178"/>
       <c r="C59" s="130" t="s">
         <v>353</v>
       </c>
@@ -7751,10 +7755,10 @@
         <v>367</v>
       </c>
       <c r="E59" s="143" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F59" s="143" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G59" s="131"/>
       <c r="H59" s="132" t="s">
@@ -7775,18 +7779,18 @@
       <c r="A60" s="1">
         <v>56</v>
       </c>
-      <c r="B60" s="169" t="s">
+      <c r="B60" s="173" t="s">
         <v>225</v>
       </c>
       <c r="C60" s="130"/>
       <c r="D60" s="130" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E60" s="143" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F60" s="143" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G60" s="131"/>
       <c r="H60" s="132"/>
@@ -7799,16 +7803,16 @@
       <c r="A61" s="1">
         <v>57</v>
       </c>
-      <c r="B61" s="159"/>
+      <c r="B61" s="168"/>
       <c r="C61" s="51"/>
       <c r="D61" s="51" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E61" s="141" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F61" s="141" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G61" s="47"/>
       <c r="H61" s="48" t="s">
@@ -7837,10 +7841,10 @@
         <v>36</v>
       </c>
       <c r="E62" s="141" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F62" s="141" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G62" s="47"/>
       <c r="H62" s="48" t="s">
@@ -7861,7 +7865,7 @@
       <c r="A63" s="1">
         <v>59</v>
       </c>
-      <c r="B63" s="158" t="s">
+      <c r="B63" s="163" t="s">
         <v>228</v>
       </c>
       <c r="C63" s="51" t="s">
@@ -7871,10 +7875,10 @@
         <v>11</v>
       </c>
       <c r="E63" s="141" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="F63" s="141" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="G63" s="47"/>
       <c r="H63" s="48" t="s">
@@ -7895,7 +7899,7 @@
       <c r="A64" s="1">
         <v>60</v>
       </c>
-      <c r="B64" s="158"/>
+      <c r="B64" s="163"/>
       <c r="C64" s="51" t="s">
         <v>229</v>
       </c>
@@ -7903,10 +7907,10 @@
         <v>230</v>
       </c>
       <c r="E64" s="141" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="F64" s="141" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="G64" s="47"/>
       <c r="H64" s="48" t="s">
@@ -7927,7 +7931,7 @@
       <c r="A65" s="1">
         <v>61</v>
       </c>
-      <c r="B65" s="158" t="s">
+      <c r="B65" s="163" t="s">
         <v>231</v>
       </c>
       <c r="C65" s="51" t="s">
@@ -7937,10 +7941,10 @@
         <v>233</v>
       </c>
       <c r="E65" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F65" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G65" s="47"/>
       <c r="H65" s="48" t="s">
@@ -7961,7 +7965,7 @@
       <c r="A66" s="1">
         <v>62</v>
       </c>
-      <c r="B66" s="158"/>
+      <c r="B66" s="163"/>
       <c r="C66" s="51" t="s">
         <v>234</v>
       </c>
@@ -7969,10 +7973,10 @@
         <v>235</v>
       </c>
       <c r="E66" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F66" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G66" s="47"/>
       <c r="H66" s="48" t="s">
@@ -7993,7 +7997,7 @@
       <c r="A67" s="1">
         <v>63</v>
       </c>
-      <c r="B67" s="158"/>
+      <c r="B67" s="163"/>
       <c r="C67" s="51" t="s">
         <v>236</v>
       </c>
@@ -8001,10 +8005,10 @@
         <v>237</v>
       </c>
       <c r="E67" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F67" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G67" s="47"/>
       <c r="H67" s="48" t="s">
@@ -8025,7 +8029,7 @@
       <c r="A68" s="1">
         <v>64</v>
       </c>
-      <c r="B68" s="158"/>
+      <c r="B68" s="163"/>
       <c r="C68" s="51" t="s">
         <v>238</v>
       </c>
@@ -8033,10 +8037,10 @@
         <v>239</v>
       </c>
       <c r="E68" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F68" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G68" s="47"/>
       <c r="H68" s="48" t="s">
@@ -8057,7 +8061,7 @@
       <c r="A69" s="1">
         <v>65</v>
       </c>
-      <c r="B69" s="158"/>
+      <c r="B69" s="163"/>
       <c r="C69" s="51" t="s">
         <v>240</v>
       </c>
@@ -8065,10 +8069,10 @@
         <v>9</v>
       </c>
       <c r="E69" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F69" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G69" s="47"/>
       <c r="H69" s="48" t="s">
@@ -8089,7 +8093,7 @@
       <c r="A70" s="1">
         <v>66</v>
       </c>
-      <c r="B70" s="158"/>
+      <c r="B70" s="163"/>
       <c r="C70" s="51" t="s">
         <v>241</v>
       </c>
@@ -8097,10 +8101,10 @@
         <v>242</v>
       </c>
       <c r="E70" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F70" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G70" s="47"/>
       <c r="H70" s="48" t="s">
@@ -8121,7 +8125,7 @@
       <c r="A71" s="1">
         <v>67</v>
       </c>
-      <c r="B71" s="158"/>
+      <c r="B71" s="163"/>
       <c r="C71" s="51" t="s">
         <v>243</v>
       </c>
@@ -8129,10 +8133,10 @@
         <v>244</v>
       </c>
       <c r="E71" s="141" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F71" s="141" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G71" s="47"/>
       <c r="H71" s="48" t="s">
@@ -8161,10 +8165,10 @@
         <v>246</v>
       </c>
       <c r="E72" s="141" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F72" s="141" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="G72" s="47"/>
       <c r="H72" s="48" t="s">
@@ -8193,10 +8197,10 @@
         <v>248</v>
       </c>
       <c r="E73" s="141" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F73" s="141" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G73" s="47"/>
       <c r="H73" s="48" t="s">
@@ -8225,10 +8229,10 @@
         <v>250</v>
       </c>
       <c r="E74" s="141" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F74" s="141" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G74" s="47"/>
       <c r="H74" s="48" t="s">
@@ -8257,10 +8261,10 @@
         <v>12</v>
       </c>
       <c r="E75" s="141" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F75" s="141" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G75" s="47"/>
       <c r="H75" s="48" t="s">
@@ -8289,10 +8293,10 @@
         <v>253</v>
       </c>
       <c r="E76" s="141" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F76" s="141" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G76" s="47"/>
       <c r="H76" s="48" t="s">
@@ -8321,10 +8325,10 @@
         <v>255</v>
       </c>
       <c r="E77" s="141" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F77" s="141" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G77" s="47"/>
       <c r="H77" s="48" t="s">
@@ -8353,10 +8357,10 @@
         <v>257</v>
       </c>
       <c r="E78" s="141" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="F78" s="141" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="G78" s="47"/>
       <c r="H78" s="48" t="s">
@@ -8385,10 +8389,10 @@
         <v>259</v>
       </c>
       <c r="E79" s="144" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F79" s="144" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="G79" s="55"/>
       <c r="H79" s="48" t="s">
@@ -8409,7 +8413,7 @@
       <c r="A80" s="1">
         <v>76</v>
       </c>
-      <c r="B80" s="169" t="s">
+      <c r="B80" s="173" t="s">
         <v>260</v>
       </c>
       <c r="C80" s="54" t="s">
@@ -8419,10 +8423,10 @@
         <v>262</v>
       </c>
       <c r="E80" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F80" s="144" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G80" s="55"/>
       <c r="H80" s="48" t="s">
@@ -8443,7 +8447,7 @@
       <c r="A81" s="1">
         <v>77</v>
       </c>
-      <c r="B81" s="171"/>
+      <c r="B81" s="174"/>
       <c r="C81" s="54" t="s">
         <v>263</v>
       </c>
@@ -8451,10 +8455,10 @@
         <v>264</v>
       </c>
       <c r="E81" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F81" s="144" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G81" s="55"/>
       <c r="H81" s="48" t="s">
@@ -8475,7 +8479,7 @@
       <c r="A82" s="1">
         <v>78</v>
       </c>
-      <c r="B82" s="159"/>
+      <c r="B82" s="168"/>
       <c r="C82" s="54" t="s">
         <v>265</v>
       </c>
@@ -8483,10 +8487,10 @@
         <v>266</v>
       </c>
       <c r="E82" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F82" s="144" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G82" s="55"/>
       <c r="H82" s="48" t="s">
@@ -8507,20 +8511,20 @@
       <c r="A83" s="1">
         <v>79</v>
       </c>
-      <c r="B83" s="169" t="s">
+      <c r="B83" s="173" t="s">
         <v>267</v>
       </c>
       <c r="C83" s="54" t="s">
         <v>268</v>
       </c>
       <c r="D83" s="54" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E83" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F83" s="144" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G83" s="55"/>
       <c r="H83" s="48" t="s">
@@ -8541,18 +8545,18 @@
       <c r="A84" s="1">
         <v>80</v>
       </c>
-      <c r="B84" s="171"/>
+      <c r="B84" s="174"/>
       <c r="C84" s="54" t="s">
         <v>269</v>
       </c>
       <c r="D84" s="54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E84" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F84" s="144" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G84" s="55"/>
       <c r="H84" s="48" t="s">
@@ -8573,18 +8577,18 @@
       <c r="A85" s="1">
         <v>81</v>
       </c>
-      <c r="B85" s="171"/>
+      <c r="B85" s="174"/>
       <c r="C85" s="54" t="s">
         <v>270</v>
       </c>
       <c r="D85" s="54" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E85" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F85" s="144" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G85" s="55"/>
       <c r="H85" s="48" t="s">
@@ -8605,20 +8609,20 @@
       <c r="A86" s="1">
         <v>82</v>
       </c>
-      <c r="B86" s="169" t="s">
+      <c r="B86" s="173" t="s">
         <v>360</v>
       </c>
       <c r="C86" s="54" t="s">
         <v>358</v>
       </c>
       <c r="D86" s="54" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E86" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F86" s="144" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G86" s="55"/>
       <c r="H86" s="48" t="s">
@@ -8639,18 +8643,18 @@
       <c r="A87" s="1">
         <v>83</v>
       </c>
-      <c r="B87" s="159"/>
+      <c r="B87" s="168"/>
       <c r="C87" s="54" t="s">
         <v>359</v>
       </c>
       <c r="D87" s="54" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E87" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F87" s="144" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G87" s="55"/>
       <c r="H87" s="48" t="s">
@@ -8671,20 +8675,20 @@
       <c r="A88" s="1">
         <v>84</v>
       </c>
-      <c r="B88" s="169" t="s">
+      <c r="B88" s="173" t="s">
         <v>379</v>
       </c>
       <c r="C88" s="54" t="s">
         <v>384</v>
       </c>
       <c r="D88" s="54" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E88" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F88" s="144" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G88" s="55"/>
       <c r="H88" s="48" t="s">
@@ -8705,7 +8709,7 @@
       <c r="A89" s="1">
         <v>85</v>
       </c>
-      <c r="B89" s="159"/>
+      <c r="B89" s="168"/>
       <c r="C89" s="54" t="s">
         <v>382</v>
       </c>
@@ -8713,10 +8717,10 @@
         <v>383</v>
       </c>
       <c r="E89" s="144" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F89" s="144" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G89" s="55"/>
       <c r="H89" s="48" t="s">
@@ -8745,10 +8749,10 @@
         <v>408</v>
       </c>
       <c r="E90" s="144" t="s">
+        <v>466</v>
+      </c>
+      <c r="F90" s="144" t="s">
         <v>468</v>
-      </c>
-      <c r="F90" s="144" t="s">
-        <v>470</v>
       </c>
       <c r="G90" s="55"/>
       <c r="H90" s="48"/>
@@ -8761,7 +8765,7 @@
       <c r="A91" s="1">
         <v>87</v>
       </c>
-      <c r="B91" s="169" t="s">
+      <c r="B91" s="173" t="s">
         <v>385</v>
       </c>
       <c r="C91" s="54" t="s">
@@ -8771,10 +8775,10 @@
         <v>388</v>
       </c>
       <c r="E91" s="144" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F91" s="144" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G91" s="55"/>
       <c r="H91" s="48"/>
@@ -8787,7 +8791,7 @@
       <c r="A92" s="1">
         <v>88</v>
       </c>
-      <c r="B92" s="170"/>
+      <c r="B92" s="175"/>
       <c r="C92" s="56" t="s">
         <v>387</v>
       </c>
@@ -8795,10 +8799,10 @@
         <v>389</v>
       </c>
       <c r="E92" s="145" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F92" s="145" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G92" s="57"/>
       <c r="H92" s="58"/>
@@ -8942,18 +8946,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B6:B22"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B44:B45"/>
     <mergeCell ref="B91:B92"/>
     <mergeCell ref="B65:B71"/>
     <mergeCell ref="B63:B64"/>
@@ -8966,6 +8958,18 @@
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="B88:B89"/>
     <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B6:B22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H23:K23 K1:K2 H1:J1048576 K4:K1048576 H88:K90">
@@ -9052,7 +9056,7 @@
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="168" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -9076,8 +9080,8 @@
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="158"/>
-      <c r="C6" s="164" t="s">
+      <c r="B6" s="163"/>
+      <c r="C6" s="157" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -9100,8 +9104,8 @@
       </c>
     </row>
     <row r="7" spans="2:11" s="121" customFormat="1">
-      <c r="B7" s="158"/>
-      <c r="C7" s="164"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="157"/>
       <c r="D7" s="114" t="s">
         <v>2</v>
       </c>
@@ -9118,7 +9122,7 @@
       <c r="K7" s="120"/>
     </row>
     <row r="8" spans="2:11" s="121" customFormat="1">
-      <c r="B8" s="158" t="s">
+      <c r="B8" s="163" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="114" t="s">
@@ -9140,7 +9144,7 @@
       <c r="K8" s="120"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="158"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="13" t="s">
         <v>51</v>
       </c>
@@ -9162,7 +9166,7 @@
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="158" t="s">
+      <c r="B10" s="163" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -9188,7 +9192,7 @@
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="158"/>
+      <c r="B11" s="163"/>
       <c r="C11" s="13" t="s">
         <v>51</v>
       </c>
@@ -9210,10 +9214,10 @@
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="158" t="s">
+      <c r="B12" s="163" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="163" t="s">
+      <c r="C12" s="160" t="s">
         <v>69</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -9236,8 +9240,8 @@
       </c>
     </row>
     <row r="13" spans="2:11" s="121" customFormat="1">
-      <c r="B13" s="158"/>
-      <c r="C13" s="163"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="160"/>
       <c r="D13" s="114" t="s">
         <v>60</v>
       </c>
@@ -9252,8 +9256,8 @@
       <c r="K13" s="120"/>
     </row>
     <row r="14" spans="2:11" ht="25.5">
-      <c r="B14" s="158"/>
-      <c r="C14" s="163"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="160"/>
       <c r="D14" s="13" t="s">
         <v>47</v>
       </c>
@@ -9272,8 +9276,8 @@
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="158"/>
-      <c r="C15" s="163" t="s">
+      <c r="B15" s="163"/>
+      <c r="C15" s="160" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -9294,8 +9298,8 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="25.5">
-      <c r="B16" s="158"/>
-      <c r="C16" s="164"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="157"/>
       <c r="D16" s="13" t="s">
         <v>47</v>
       </c>
@@ -9314,7 +9318,7 @@
       </c>
     </row>
     <row r="17" spans="2:11" s="121" customFormat="1">
-      <c r="B17" s="161" t="s">
+      <c r="B17" s="165" t="s">
         <v>77</v>
       </c>
       <c r="C17" s="114" t="s">
@@ -9336,8 +9340,8 @@
       <c r="K17" s="120"/>
     </row>
     <row r="18" spans="2:11" ht="25.5">
-      <c r="B18" s="161"/>
-      <c r="C18" s="164" t="s">
+      <c r="B18" s="165"/>
+      <c r="C18" s="157" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -9360,8 +9364,8 @@
       </c>
     </row>
     <row r="19" spans="2:11" ht="25.5">
-      <c r="B19" s="161"/>
-      <c r="C19" s="164"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="157"/>
       <c r="D19" s="13" t="s">
         <v>52</v>
       </c>
@@ -9382,7 +9386,7 @@
       </c>
     </row>
     <row r="20" spans="2:11" ht="25.5">
-      <c r="B20" s="161"/>
+      <c r="B20" s="165"/>
       <c r="C20" s="19" t="s">
         <v>82</v>
       </c>
@@ -9406,7 +9410,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" s="121" customFormat="1">
-      <c r="B21" s="161"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="114" t="s">
         <v>84</v>
       </c>
@@ -9446,10 +9450,10 @@
       <c r="K22" s="128"/>
     </row>
     <row r="23" spans="2:11" hidden="1">
-      <c r="B23" s="165" t="s">
+      <c r="B23" s="156" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="167" t="s">
+      <c r="C23" s="159" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -9468,8 +9472,8 @@
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" hidden="1">
-      <c r="B24" s="164"/>
-      <c r="C24" s="163"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="160"/>
       <c r="D24" s="13" t="s">
         <v>47</v>
       </c>
@@ -9484,8 +9488,8 @@
       <c r="K24" s="17"/>
     </row>
     <row r="25" spans="2:11" ht="27" hidden="1" customHeight="1">
-      <c r="B25" s="164"/>
-      <c r="C25" s="163" t="s">
+      <c r="B25" s="157"/>
+      <c r="C25" s="160" t="s">
         <v>105</v>
       </c>
       <c r="D25" s="13" t="s">
@@ -9504,8 +9508,8 @@
       <c r="K25" s="17"/>
     </row>
     <row r="26" spans="2:11" hidden="1">
-      <c r="B26" s="164"/>
-      <c r="C26" s="163"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="160"/>
       <c r="D26" s="13" t="s">
         <v>47</v>
       </c>
@@ -9520,8 +9524,8 @@
       <c r="K26" s="17"/>
     </row>
     <row r="27" spans="2:11" ht="27" hidden="1" customHeight="1">
-      <c r="B27" s="164"/>
-      <c r="C27" s="163" t="s">
+      <c r="B27" s="157"/>
+      <c r="C27" s="160" t="s">
         <v>107</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -9542,8 +9546,8 @@
       </c>
     </row>
     <row r="28" spans="2:11" hidden="1">
-      <c r="B28" s="164"/>
-      <c r="C28" s="163"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="160"/>
       <c r="D28" s="13" t="s">
         <v>47</v>
       </c>
@@ -9558,8 +9562,8 @@
       <c r="K28" s="17"/>
     </row>
     <row r="29" spans="2:11" ht="27" hidden="1" customHeight="1">
-      <c r="B29" s="164"/>
-      <c r="C29" s="163" t="s">
+      <c r="B29" s="157"/>
+      <c r="C29" s="160" t="s">
         <v>109</v>
       </c>
       <c r="D29" s="13" t="s">
@@ -9580,8 +9584,8 @@
       </c>
     </row>
     <row r="30" spans="2:11" hidden="1">
-      <c r="B30" s="164"/>
-      <c r="C30" s="163"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="160"/>
       <c r="D30" s="13" t="s">
         <v>47</v>
       </c>
@@ -9596,8 +9600,8 @@
       <c r="K30" s="17"/>
     </row>
     <row r="31" spans="2:11" ht="27" hidden="1" customHeight="1">
-      <c r="B31" s="164"/>
-      <c r="C31" s="163" t="s">
+      <c r="B31" s="157"/>
+      <c r="C31" s="160" t="s">
         <v>111</v>
       </c>
       <c r="D31" s="13" t="s">
@@ -9616,8 +9620,8 @@
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="2:11" hidden="1">
-      <c r="B32" s="164"/>
-      <c r="C32" s="163"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="160"/>
       <c r="D32" s="13" t="s">
         <v>47</v>
       </c>
@@ -9631,8 +9635,8 @@
       <c r="J32" s="16"/>
     </row>
     <row r="33" spans="2:10" ht="27" hidden="1" customHeight="1">
-      <c r="B33" s="164"/>
-      <c r="C33" s="163" t="s">
+      <c r="B33" s="157"/>
+      <c r="C33" s="160" t="s">
         <v>113</v>
       </c>
       <c r="D33" s="13" t="s">
@@ -9650,8 +9654,8 @@
       <c r="J33" s="16"/>
     </row>
     <row r="34" spans="2:10" ht="17.25" hidden="1" customHeight="1" thickBot="1">
-      <c r="B34" s="166"/>
-      <c r="C34" s="168"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="161"/>
       <c r="D34" s="20" t="s">
         <v>47</v>
       </c>
@@ -9793,6 +9797,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="C15:C16"/>
@@ -9806,11 +9815,6 @@
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G1:J1048576">
@@ -9932,7 +9936,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="170" t="s">
         <v>134</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -9956,7 +9960,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="178"/>
+      <c r="B7" s="172"/>
       <c r="C7" s="14" t="s">
         <v>137</v>
       </c>
@@ -9978,7 +9982,7 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="178"/>
+      <c r="B8" s="172"/>
       <c r="C8" s="51" t="s">
         <v>139</v>
       </c>
@@ -10000,7 +10004,7 @@
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="178"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="51" t="s">
         <v>141</v>
       </c>
@@ -10024,7 +10028,7 @@
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="178"/>
+      <c r="B10" s="172"/>
       <c r="C10" s="51" t="s">
         <v>144</v>
       </c>
@@ -10046,7 +10050,7 @@
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="178"/>
+      <c r="B11" s="172"/>
       <c r="C11" s="51" t="s">
         <v>146</v>
       </c>
@@ -10068,7 +10072,7 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="178"/>
+      <c r="B12" s="172"/>
       <c r="C12" s="51" t="s">
         <v>148</v>
       </c>
@@ -10090,7 +10094,7 @@
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="178"/>
+      <c r="B13" s="172"/>
       <c r="C13" s="51" t="s">
         <v>150</v>
       </c>
@@ -10114,7 +10118,7 @@
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="178"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="14" t="s">
         <v>153</v>
       </c>
@@ -10136,7 +10140,7 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="178"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="51" t="s">
         <v>155</v>
       </c>
@@ -10158,7 +10162,7 @@
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="178"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="51" t="s">
         <v>157</v>
       </c>
@@ -10180,7 +10184,7 @@
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="178"/>
+      <c r="B17" s="172"/>
       <c r="C17" s="51" t="s">
         <v>159</v>
       </c>
@@ -10202,7 +10206,7 @@
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="178"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="51" t="s">
         <v>161</v>
       </c>
@@ -10224,7 +10228,7 @@
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="178"/>
+      <c r="B19" s="172"/>
       <c r="C19" s="51" t="s">
         <v>164</v>
       </c>
@@ -10243,7 +10247,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.5" customHeight="1">
-      <c r="B20" s="178"/>
+      <c r="B20" s="172"/>
       <c r="C20" s="51" t="s">
         <v>394</v>
       </c>
@@ -10258,7 +10262,7 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" customHeight="1">
-      <c r="B21" s="178"/>
+      <c r="B21" s="172"/>
       <c r="C21" s="51" t="s">
         <v>411</v>
       </c>
@@ -10273,7 +10277,7 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" customHeight="1">
-      <c r="B22" s="177"/>
+      <c r="B22" s="171"/>
       <c r="C22" s="51" t="s">
         <v>409</v>
       </c>
@@ -10291,7 +10295,7 @@
       <c r="A23" s="1">
         <v>16</v>
       </c>
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="170" t="s">
         <v>166</v>
       </c>
       <c r="C23" s="51" t="s">
@@ -10315,7 +10319,7 @@
       <c r="A24" s="1">
         <v>17</v>
       </c>
-      <c r="B24" s="177"/>
+      <c r="B24" s="171"/>
       <c r="C24" s="51" t="s">
         <v>167</v>
       </c>
@@ -10361,7 +10365,7 @@
       <c r="A26" s="1">
         <v>19</v>
       </c>
-      <c r="B26" s="158" t="s">
+      <c r="B26" s="163" t="s">
         <v>327</v>
       </c>
       <c r="C26" s="51" t="s">
@@ -10385,7 +10389,7 @@
       <c r="A27" s="1">
         <v>20</v>
       </c>
-      <c r="B27" s="158"/>
+      <c r="B27" s="163"/>
       <c r="C27" s="51" t="s">
         <v>177</v>
       </c>
@@ -10407,7 +10411,7 @@
       <c r="A28" s="1">
         <v>21</v>
       </c>
-      <c r="B28" s="169" t="s">
+      <c r="B28" s="173" t="s">
         <v>137</v>
       </c>
       <c r="C28" s="51" t="s">
@@ -10431,7 +10435,7 @@
       <c r="A29" s="1">
         <v>22</v>
       </c>
-      <c r="B29" s="159"/>
+      <c r="B29" s="168"/>
       <c r="C29" s="51" t="s">
         <v>181</v>
       </c>
@@ -10453,7 +10457,7 @@
       <c r="A30" s="1">
         <v>23</v>
       </c>
-      <c r="B30" s="169" t="s">
+      <c r="B30" s="173" t="s">
         <v>183</v>
       </c>
       <c r="C30" s="51" t="s">
@@ -10477,7 +10481,7 @@
       <c r="A31" s="1">
         <v>24</v>
       </c>
-      <c r="B31" s="171"/>
+      <c r="B31" s="174"/>
       <c r="C31" s="51" t="s">
         <v>186</v>
       </c>
@@ -10499,7 +10503,7 @@
       <c r="A32" s="1">
         <v>25</v>
       </c>
-      <c r="B32" s="171"/>
+      <c r="B32" s="174"/>
       <c r="C32" s="51" t="s">
         <v>188</v>
       </c>
@@ -10521,7 +10525,7 @@
       <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B33" s="169" t="s">
+      <c r="B33" s="173" t="s">
         <v>190</v>
       </c>
       <c r="C33" s="51" t="s">
@@ -10545,7 +10549,7 @@
       <c r="A34" s="1">
         <v>27</v>
       </c>
-      <c r="B34" s="171"/>
+      <c r="B34" s="174"/>
       <c r="C34" s="51" t="s">
         <v>193</v>
       </c>
@@ -10567,7 +10571,7 @@
       <c r="A35" s="1">
         <v>28</v>
       </c>
-      <c r="B35" s="171"/>
+      <c r="B35" s="174"/>
       <c r="C35" s="51" t="s">
         <v>195</v>
       </c>
@@ -10589,7 +10593,7 @@
       <c r="A36" s="1">
         <v>29</v>
       </c>
-      <c r="B36" s="169" t="s">
+      <c r="B36" s="173" t="s">
         <v>197</v>
       </c>
       <c r="C36" s="51" t="s">
@@ -10613,7 +10617,7 @@
       <c r="A37" s="1">
         <v>30</v>
       </c>
-      <c r="B37" s="171"/>
+      <c r="B37" s="174"/>
       <c r="C37" s="51" t="s">
         <v>200</v>
       </c>
@@ -10635,7 +10639,7 @@
       <c r="A38" s="1">
         <v>31</v>
       </c>
-      <c r="B38" s="171"/>
+      <c r="B38" s="174"/>
       <c r="C38" s="51" t="s">
         <v>202</v>
       </c>
@@ -10657,7 +10661,7 @@
       <c r="A39" s="1">
         <v>32</v>
       </c>
-      <c r="B39" s="169" t="s">
+      <c r="B39" s="173" t="s">
         <v>204</v>
       </c>
       <c r="C39" s="51" t="s">
@@ -10681,7 +10685,7 @@
       <c r="A40" s="1">
         <v>33</v>
       </c>
-      <c r="B40" s="171"/>
+      <c r="B40" s="174"/>
       <c r="C40" s="51" t="s">
         <v>206</v>
       </c>
@@ -10703,7 +10707,7 @@
       <c r="A41" s="1">
         <v>34</v>
       </c>
-      <c r="B41" s="169" t="s">
+      <c r="B41" s="173" t="s">
         <v>208</v>
       </c>
       <c r="C41" s="51" t="s">
@@ -10727,7 +10731,7 @@
       <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B42" s="171"/>
+      <c r="B42" s="174"/>
       <c r="C42" s="51" t="s">
         <v>211</v>
       </c>
@@ -10749,7 +10753,7 @@
       <c r="A43" s="1">
         <v>36</v>
       </c>
-      <c r="B43" s="171"/>
+      <c r="B43" s="174"/>
       <c r="C43" s="51" t="s">
         <v>200</v>
       </c>
@@ -10771,7 +10775,7 @@
       <c r="A44" s="1">
         <v>37</v>
       </c>
-      <c r="B44" s="171"/>
+      <c r="B44" s="174"/>
       <c r="C44" s="51" t="s">
         <v>214</v>
       </c>
@@ -10793,7 +10797,7 @@
       <c r="A45" s="1">
         <v>38</v>
       </c>
-      <c r="B45" s="158" t="s">
+      <c r="B45" s="163" t="s">
         <v>216</v>
       </c>
       <c r="C45" s="51" t="s">
@@ -10817,7 +10821,7 @@
       <c r="A46" s="1">
         <v>39</v>
       </c>
-      <c r="B46" s="158"/>
+      <c r="B46" s="163"/>
       <c r="C46" s="51" t="s">
         <v>219</v>
       </c>
@@ -10839,7 +10843,7 @@
       <c r="A47" s="1">
         <v>40</v>
       </c>
-      <c r="B47" s="158"/>
+      <c r="B47" s="163"/>
       <c r="C47" s="51" t="s">
         <v>221</v>
       </c>
@@ -10883,7 +10887,7 @@
       <c r="A49" s="129">
         <v>42</v>
       </c>
-      <c r="B49" s="172" t="s">
+      <c r="B49" s="176" t="s">
         <v>346</v>
       </c>
       <c r="C49" s="130" t="s">
@@ -10909,7 +10913,7 @@
       <c r="A50" s="129">
         <v>43</v>
       </c>
-      <c r="B50" s="173"/>
+      <c r="B50" s="177"/>
       <c r="C50" s="130" t="s">
         <v>349</v>
       </c>
@@ -10931,7 +10935,7 @@
       <c r="A51" s="129">
         <v>44</v>
       </c>
-      <c r="B51" s="173"/>
+      <c r="B51" s="177"/>
       <c r="C51" s="130" t="s">
         <v>351</v>
       </c>
@@ -10953,7 +10957,7 @@
       <c r="A52" s="129">
         <v>45</v>
       </c>
-      <c r="B52" s="174"/>
+      <c r="B52" s="178"/>
       <c r="C52" s="130" t="s">
         <v>353</v>
       </c>
@@ -11021,7 +11025,7 @@
       <c r="A55" s="1">
         <v>48</v>
       </c>
-      <c r="B55" s="158" t="s">
+      <c r="B55" s="163" t="s">
         <v>228</v>
       </c>
       <c r="C55" s="51" t="s">
@@ -11045,7 +11049,7 @@
       <c r="A56" s="1">
         <v>49</v>
       </c>
-      <c r="B56" s="158"/>
+      <c r="B56" s="163"/>
       <c r="C56" s="51" t="s">
         <v>229</v>
       </c>
@@ -11067,7 +11071,7 @@
       <c r="A57" s="1">
         <v>50</v>
       </c>
-      <c r="B57" s="158" t="s">
+      <c r="B57" s="163" t="s">
         <v>231</v>
       </c>
       <c r="C57" s="51" t="s">
@@ -11091,7 +11095,7 @@
       <c r="A58" s="1">
         <v>51</v>
       </c>
-      <c r="B58" s="158"/>
+      <c r="B58" s="163"/>
       <c r="C58" s="51" t="s">
         <v>234</v>
       </c>
@@ -11113,7 +11117,7 @@
       <c r="A59" s="1">
         <v>52</v>
       </c>
-      <c r="B59" s="158"/>
+      <c r="B59" s="163"/>
       <c r="C59" s="51" t="s">
         <v>236</v>
       </c>
@@ -11135,7 +11139,7 @@
       <c r="A60" s="1">
         <v>53</v>
       </c>
-      <c r="B60" s="158"/>
+      <c r="B60" s="163"/>
       <c r="C60" s="51" t="s">
         <v>238</v>
       </c>
@@ -11157,7 +11161,7 @@
       <c r="A61" s="1">
         <v>54</v>
       </c>
-      <c r="B61" s="158"/>
+      <c r="B61" s="163"/>
       <c r="C61" s="51" t="s">
         <v>240</v>
       </c>
@@ -11179,7 +11183,7 @@
       <c r="A62" s="1">
         <v>55</v>
       </c>
-      <c r="B62" s="158"/>
+      <c r="B62" s="163"/>
       <c r="C62" s="51" t="s">
         <v>241</v>
       </c>
@@ -11201,7 +11205,7 @@
       <c r="A63" s="1">
         <v>56</v>
       </c>
-      <c r="B63" s="158"/>
+      <c r="B63" s="163"/>
       <c r="C63" s="51" t="s">
         <v>243</v>
       </c>
@@ -11399,7 +11403,7 @@
       <c r="A72" s="1">
         <v>65</v>
       </c>
-      <c r="B72" s="169" t="s">
+      <c r="B72" s="173" t="s">
         <v>260</v>
       </c>
       <c r="C72" s="54" t="s">
@@ -11423,7 +11427,7 @@
       <c r="A73" s="1">
         <v>66</v>
       </c>
-      <c r="B73" s="171"/>
+      <c r="B73" s="174"/>
       <c r="C73" s="54" t="s">
         <v>263</v>
       </c>
@@ -11445,7 +11449,7 @@
       <c r="A74" s="1">
         <v>67</v>
       </c>
-      <c r="B74" s="169" t="s">
+      <c r="B74" s="173" t="s">
         <v>364</v>
       </c>
       <c r="C74" s="54" t="s">
@@ -11469,7 +11473,7 @@
       <c r="A75" s="1">
         <v>68</v>
       </c>
-      <c r="B75" s="171"/>
+      <c r="B75" s="174"/>
       <c r="C75" s="54" t="s">
         <v>269</v>
       </c>
@@ -11491,7 +11495,7 @@
       <c r="A76" s="1">
         <v>69</v>
       </c>
-      <c r="B76" s="171"/>
+      <c r="B76" s="174"/>
       <c r="C76" s="54" t="s">
         <v>270</v>
       </c>
@@ -11513,7 +11517,7 @@
       <c r="A77" s="1">
         <v>70</v>
       </c>
-      <c r="B77" s="169" t="s">
+      <c r="B77" s="173" t="s">
         <v>360</v>
       </c>
       <c r="C77" s="54" t="s">
@@ -11537,7 +11541,7 @@
       <c r="A78" s="1">
         <v>71</v>
       </c>
-      <c r="B78" s="159"/>
+      <c r="B78" s="168"/>
       <c r="C78" s="54" t="s">
         <v>359</v>
       </c>
@@ -11752,6 +11756,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B63"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B76"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B47"/>
@@ -11763,12 +11773,6 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B63"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B76"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F83:I1048576 F1:I81">
@@ -11825,29 +11829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_xad6c__xbd84_ xmlns="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568">QA 업무공유</_xad6c__xbd84_>
-    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_xb300__xc0c1__x0020__xadf8__xb8f9_ xmlns="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568" xsi:nil="true"/>
-    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x010100347EF733F8488B44B6166A12BD2DCC35" ma:contentTypeVersion="7" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="f32a2cf0b8dcac8198a1dea87630ec13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="accedb8ad30dc317877b8d34566b5190" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11956,31 +11937,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{464C72DE-A2DD-417A-A227-849B7750E283}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E9BBC0-E9CB-4222-8FDE-BCB95C70D77D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_xad6c__xbd84_ xmlns="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568">QA 업무공유</_xad6c__xbd84_>
+    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_xb300__xc0c1__x0020__xadf8__xb8f9_ xmlns="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568" xsi:nil="true"/>
+    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531C7103-68AF-4123-B4AB-98A3B019F9A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11996,4 +11976,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E9BBC0-E9CB-4222-8FDE-BCB95C70D77D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{464C72DE-A2DD-417A-A227-849B7750E283}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e7cdbefa-3dae-44e9-b4a7-dc79b6d35568"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>